<commit_message>
Quick save to age table
</commit_message>
<xml_diff>
--- a/AgeTable.xlsx
+++ b/AgeTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trezendes\projects\AgeOfTheDoctor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BB94BA-83F9-4194-AC10-19E4D6B0AB3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FEC64C-86E0-478C-9F66-D492EE0BA281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{65FED239-CF6D-4748-B1D0-82DAE2B993D6}"/>
   </bookViews>
@@ -401,8 +401,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C77E90DF-C573-4D57-BADA-2537C79A91D3}" name="Table1" displayName="Table1" ref="A1:L18" totalsRowShown="0" headerRowDxfId="9" dataDxfId="10">
   <autoFilter ref="A1:L18" xr:uid="{C77E90DF-C573-4D57-BADA-2537C79A91D3}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L17">
-    <sortCondition ref="C1:C17"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L18">
+    <sortCondition ref="C1:C18"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{A970DF76-AF80-47BA-BEF4-C4ADF93E14E6}" name="Actor" dataDxfId="13"/>
@@ -742,7 +742,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="I18" activeCellId="7" sqref="F14 I14 F15 I15 F17 I17 F18 I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,7 +835,7 @@
         <v>214.79</v>
       </c>
       <c r="J2" s="1" t="str">
-        <f t="shared" ref="J2:J18" si="0">DATEDIF($B2,$D2, "y")&amp;" years, "
+        <f>DATEDIF($B2,$D2, "y")&amp;" years, "
 &amp;DATEDIF($B2,$D2, "ym")&amp;" months, "
 &amp;$D2-DATE(YEAR($D2), MONTH($D2), 1)&amp;" days"</f>
         <v>58 years, 9 months, 28 days</v>
@@ -885,7 +885,9 @@
         <v>179.85</v>
       </c>
       <c r="J3" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>DATEDIF($B3,$D3, "y")&amp;" years, "
+&amp;DATEDIF($B3,$D3, "ym")&amp;" months, "
+&amp;$D3-DATE(YEAR($D3), MONTH($D3), 1)&amp;" days"</f>
         <v>49 years, 2 months, 20 days</v>
       </c>
       <c r="K3" s="1">
@@ -933,7 +935,9 @@
         <v>200.6</v>
       </c>
       <c r="J4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>DATEDIF($B4,$D4, "y")&amp;" years, "
+&amp;DATEDIF($B4,$D4, "ym")&amp;" months, "
+&amp;$D4-DATE(YEAR($D4), MONTH($D4), 1)&amp;" days"</f>
         <v>54 years, 11 months, 7 days</v>
       </c>
       <c r="K4" s="1">
@@ -981,7 +985,9 @@
         <v>172.27</v>
       </c>
       <c r="J5" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>DATEDIF($B5,$D5, "y")&amp;" years, "
+&amp;DATEDIF($B5,$D5, "ym")&amp;" months, "
+&amp;$D5-DATE(YEAR($D5), MONTH($D5), 1)&amp;" days"</f>
         <v>47 years, 2 months, 20 days</v>
       </c>
       <c r="K5" s="1">
@@ -1029,7 +1035,9 @@
         <v>120.26</v>
       </c>
       <c r="J6" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>DATEDIF($B6,$D6, "y")&amp;" years, "
+&amp;DATEDIF($B6,$D6, "ym")&amp;" months, "
+&amp;$D6-DATE(YEAR($D6), MONTH($D6), 1)&amp;" days"</f>
         <v>32 years, 11 months, 15 days</v>
       </c>
       <c r="K6" s="1">
@@ -1077,7 +1085,9 @@
         <v>161.62</v>
       </c>
       <c r="J7" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>DATEDIF($B7,$D7, "y")&amp;" years, "
+&amp;DATEDIF($B7,$D7, "ym")&amp;" months, "
+&amp;$D7-DATE(YEAR($D7), MONTH($D7), 1)&amp;" days"</f>
         <v>44 years, 2 months, 6 days</v>
       </c>
       <c r="K7" s="1">
@@ -1125,7 +1135,9 @@
         <v>192.59</v>
       </c>
       <c r="J8" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>DATEDIF($B8,$D8, "y")&amp;" years, "
+&amp;DATEDIF($B8,$D8, "ym")&amp;" months, "
+&amp;$D8-DATE(YEAR($D8), MONTH($D8), 1)&amp;" days"</f>
         <v>52 years, 8 months, 11 days</v>
       </c>
       <c r="K8" s="1">
@@ -1173,7 +1185,9 @@
         <v>197.24</v>
       </c>
       <c r="J9" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>DATEDIF($B9,$D9, "y")&amp;" years, "
+&amp;DATEDIF($B9,$D9, "ym")&amp;" months, "
+&amp;$D9-DATE(YEAR($D9), MONTH($D9), 1)&amp;" days"</f>
         <v>54 years, 0 months, 13 days</v>
       </c>
       <c r="K9" s="1">
@@ -1221,7 +1235,9 @@
         <v>150.97999999999999</v>
       </c>
       <c r="J10" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>DATEDIF($B10,$D10, "y")&amp;" years, "
+&amp;DATEDIF($B10,$D10, "ym")&amp;" months, "
+&amp;$D10-DATE(YEAR($D10), MONTH($D10), 1)&amp;" days"</f>
         <v>41 years, 4 months, 17 days</v>
       </c>
       <c r="K10" s="1">
@@ -1269,7 +1285,9 @@
         <v>141.38</v>
       </c>
       <c r="J11" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>DATEDIF($B11,$D11, "y")&amp;" years, "
+&amp;DATEDIF($B11,$D11, "ym")&amp;" months, "
+&amp;$D11-DATE(YEAR($D11), MONTH($D11), 1)&amp;" days"</f>
         <v>38 years, 8 months, 0 days</v>
       </c>
       <c r="K11" s="1">
@@ -1317,7 +1335,9 @@
         <v>116.22</v>
       </c>
       <c r="J12" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>DATEDIF($B12,$D12, "y")&amp;" years, "
+&amp;DATEDIF($B12,$D12, "ym")&amp;" months, "
+&amp;$D12-DATE(YEAR($D12), MONTH($D12), 1)&amp;" days"</f>
         <v>31 years, 9 months, 22 days</v>
       </c>
       <c r="K12" s="1">
@@ -1365,7 +1385,9 @@
         <v>269.69</v>
       </c>
       <c r="J13" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f>DATEDIF($B13,$D13, "y")&amp;" years, "
+&amp;DATEDIF($B13,$D13, "ym")&amp;" months, "
+&amp;$D13-DATE(YEAR($D13), MONTH($D13), 1)&amp;" days"</f>
         <v>73 years, 10 months, 22 days</v>
       </c>
       <c r="K13" s="4">
@@ -1413,7 +1435,9 @@
         <v>218.05</v>
       </c>
       <c r="J14" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>DATEDIF($B14,$D14, "y")&amp;" years, "
+&amp;DATEDIF($B14,$D14, "ym")&amp;" months, "
+&amp;$D14-DATE(YEAR($D14), MONTH($D14), 1)&amp;" days"</f>
         <v>59 years, 8 months, 24 days</v>
       </c>
       <c r="K14" s="1">
@@ -1461,7 +1485,9 @@
         <v>147.38</v>
       </c>
       <c r="J15" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>DATEDIF($B15,$D15, "y")&amp;" years, "
+&amp;DATEDIF($B15,$D15, "ym")&amp;" months, "
+&amp;$D15-DATE(YEAR($D15), MONTH($D15), 1)&amp;" days"</f>
         <v>40 years, 4 months, 22 days</v>
       </c>
       <c r="K15" s="1">
@@ -1509,7 +1535,9 @@
         <v>151.74</v>
       </c>
       <c r="J16" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f>DATEDIF($B16,$D16, "y")&amp;" years, "
+&amp;DATEDIF($B16,$D16, "ym")&amp;" months, "
+&amp;$D16-DATE(YEAR($D16), MONTH($D16), 1)&amp;" days"</f>
         <v>41 years, 6 months, 13 days</v>
       </c>
       <c r="K16" s="4">
@@ -1523,98 +1551,102 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B17" s="2">
-        <v>33892</v>
+        <v>26041</v>
       </c>
       <c r="C17" s="2">
+        <v>44857</v>
+      </c>
+      <c r="D17" s="2">
         <v>45269</v>
-      </c>
-      <c r="D17" s="2">
-        <v>45285</v>
       </c>
       <c r="E17" s="4">
         <f>DATEDIF($B17, $C17, "d")</f>
-        <v>11377</v>
+        <v>18816</v>
       </c>
       <c r="F17" s="4">
         <f>($E17-MIN(Table1[Youngest Portrayal (Days)]))/100</f>
-        <v>14.5</v>
-      </c>
-      <c r="G17" s="1" t="str">
+        <v>88.89</v>
+      </c>
+      <c r="G17" s="4" t="str">
         <f>DATEDIF($B17, C17, "y")&amp;" years, "
 &amp;DATEDIF($B17, C17, "ym")&amp;" months, "
 &amp;C17-DATE(YEAR(C17), MONTH(C17), 1)&amp;" days"</f>
-        <v>31 years, 1 months, 8 days</v>
-      </c>
-      <c r="H17" s="1">
+        <v>51 years, 6 months, 22 days</v>
+      </c>
+      <c r="H17" s="4">
         <f>DATEDIF($B17, $D17, "d")</f>
-        <v>11393</v>
-      </c>
-      <c r="I17" s="1">
+        <v>19228</v>
+      </c>
+      <c r="I17" s="4">
         <f>$H17/100</f>
-        <v>113.93</v>
-      </c>
-      <c r="J17" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>31 years, 2 months, 24 days</v>
-      </c>
-      <c r="K17" s="1">
+        <v>192.28</v>
+      </c>
+      <c r="J17" s="4" t="str">
+        <f>DATEDIF($B17,$D17, "y")&amp;" years, "
+&amp;DATEDIF($B17,$D17, "ym")&amp;" months, "
+&amp;$D17-DATE(YEAR($D17), MONTH($D17), 1)&amp;" days"</f>
+        <v>52 years, 7 months, 8 days</v>
+      </c>
+      <c r="K17" s="4">
         <f>_xlfn.RANK.EQ(E17, Table1[Youngest Portrayal (Days)], 1)</f>
-        <v>3</v>
-      </c>
-      <c r="L17" s="1">
+        <v>14</v>
+      </c>
+      <c r="L17" s="4">
         <f>_xlfn.RANK.EQ(H17, Table1[Oldest Portrayal (Days)], 0)</f>
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B18" s="2">
-        <v>26041</v>
+        <v>33892</v>
       </c>
       <c r="C18" s="2">
-        <v>44857</v>
+        <v>45269</v>
       </c>
       <c r="D18" s="2">
-        <v>45269</v>
+        <v>45285</v>
       </c>
       <c r="E18" s="4">
         <f>DATEDIF($B18, $C18, "d")</f>
-        <v>18816</v>
+        <v>11377</v>
       </c>
       <c r="F18" s="4">
         <f>($E18-MIN(Table1[Youngest Portrayal (Days)]))/100</f>
-        <v>88.89</v>
-      </c>
-      <c r="G18" s="4" t="str">
+        <v>14.5</v>
+      </c>
+      <c r="G18" s="1" t="str">
         <f>DATEDIF($B18, C18, "y")&amp;" years, "
 &amp;DATEDIF($B18, C18, "ym")&amp;" months, "
 &amp;C18-DATE(YEAR(C18), MONTH(C18), 1)&amp;" days"</f>
-        <v>51 years, 6 months, 22 days</v>
-      </c>
-      <c r="H18" s="4">
+        <v>31 years, 1 months, 8 days</v>
+      </c>
+      <c r="H18" s="1">
         <f>DATEDIF($B18, $D18, "d")</f>
-        <v>19228</v>
-      </c>
-      <c r="I18" s="4">
+        <v>11393</v>
+      </c>
+      <c r="I18" s="1">
         <f>$H18/100</f>
-        <v>192.28</v>
-      </c>
-      <c r="J18" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>52 years, 7 months, 8 days</v>
-      </c>
-      <c r="K18" s="4">
+        <v>113.93</v>
+      </c>
+      <c r="J18" s="1" t="str">
+        <f>DATEDIF($B18,$D18, "y")&amp;" years, "
+&amp;DATEDIF($B18,$D18, "ym")&amp;" months, "
+&amp;$D18-DATE(YEAR($D18), MONTH($D18), 1)&amp;" days"</f>
+        <v>31 years, 2 months, 24 days</v>
+      </c>
+      <c r="K18" s="1">
         <f>_xlfn.RANK.EQ(E18, Table1[Youngest Portrayal (Days)], 1)</f>
-        <v>14</v>
-      </c>
-      <c r="L18" s="4">
+        <v>3</v>
+      </c>
+      <c r="L18" s="1">
         <f>_xlfn.RANK.EQ(H18, Table1[Oldest Portrayal (Days)], 0)</f>
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>